<commit_message>
specific folders for input and output
</commit_message>
<xml_diff>
--- a/jobbfordeler/Output/Lederønsker.xlsx
+++ b/jobbfordeler/Output/Lederønsker.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>1. årsleder-opplegg</t>
   </si>
@@ -163,6 +163,9 @@
     <t>Spille cajon</t>
   </si>
   <si>
+    <t>Være forsanger</t>
+  </si>
+  <si>
     <t>Spille piano</t>
   </si>
   <si>
@@ -170,12 +173,6 @@
   </si>
   <si>
     <t>Spille trommer</t>
-  </si>
-  <si>
-    <t>Spille et instrument Susanne har glemt:__________</t>
-  </si>
-  <si>
-    <t>Være forsanger</t>
   </si>
   <si>
     <t>Bass</t>
@@ -767,87 +764,87 @@
       <c r="B2" t="s">
         <v>42</v>
       </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
       <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -887,21 +884,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -933,62 +930,62 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1023,80 +1020,80 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>74</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>76</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>79</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>80</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>81</v>
-      </c>
-      <c r="L2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>